<commit_message>
Load all tables from Excel.Labels show selected Manufactor and Fixture
</commit_message>
<xml_diff>
--- a/dataFolder/db.xlsx
+++ b/dataFolder/db.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4d61822a20a7d592/Visual Studio 2019/PROJECTS/SpareParts/dataFolder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="11_F25DC773A252ABDACC10480CE9DD75C05BDE58F6" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3FB5DD70-CBAD-4464-8CE3-8B8FB421DBE2}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="11_F25DC773A252ABDACC10480CE9DD75C05BDE58F6" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D9081E4C-C88C-49A3-89C0-6A35B5FD3AED}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spare" sheetId="1" r:id="rId1"/>
     <sheet name="Fixtures" sheetId="2" r:id="rId2"/>
-    <sheet name="STORE" sheetId="5" r:id="rId3"/>
+    <sheet name="Action" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="207">
   <si>
     <t>id_manufactor</t>
   </si>
@@ -621,6 +621,39 @@
   </si>
   <si>
     <t>FixtureType</t>
+  </si>
+  <si>
+    <t>id_pers</t>
+  </si>
+  <si>
+    <t>Personnel</t>
+  </si>
+  <si>
+    <t>Электроник</t>
+  </si>
+  <si>
+    <t>Омел</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>Илья</t>
+  </si>
+  <si>
+    <t>Пушкин</t>
+  </si>
+  <si>
+    <t>Крылов</t>
+  </si>
+  <si>
+    <t>Якин</t>
+  </si>
+  <si>
+    <t>Женя</t>
+  </si>
+  <si>
+    <t>Pers</t>
   </si>
 </sst>
 </file>
@@ -677,9 +710,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -743,6 +773,9 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
@@ -827,9 +860,20 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{42D45206-B671-4411-B18D-82942EE0FAE7}" name="Action" displayName="Action" ref="A1:L50" totalsRowShown="0">
-  <autoFilter ref="A1:L50" xr:uid="{32FC500A-6F56-4D7B-B2EB-116432F8B7B1}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E47A2296-9C2C-4020-B6DC-6F0C1AA8E787}" name="Personnel" displayName="Personnel" ref="M1:N9" totalsRowShown="0">
+  <autoFilter ref="M1:N9" xr:uid="{244D9122-7B9B-401B-BFAD-C7118176C20F}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{C3B876D2-134F-4FBF-9F5E-22F84A18E70E}" name="id_pers"/>
+    <tableColumn id="2" xr3:uid="{77FA02A3-FA72-4458-AC9E-7A0691472DDF}" name="Personnel"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{42D45206-B671-4411-B18D-82942EE0FAE7}" name="Action" displayName="Action" ref="A1:M50" totalsRowShown="0">
+  <autoFilter ref="A1:M50" xr:uid="{32FC500A-6F56-4D7B-B2EB-116432F8B7B1}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{71498E56-71D7-4893-BADB-26F4278F0FAF}" name="id_action"/>
     <tableColumn id="2" xr3:uid="{F848BE6F-3F60-4341-AAA8-A8FB3F2C82ED}" name="Date" dataDxfId="3">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
@@ -838,12 +882,13 @@
     <tableColumn id="4" xr3:uid="{0E235997-4E11-415E-9C07-8541C9EFCF48}" name="Type"/>
     <tableColumn id="5" xr3:uid="{B5773653-3727-4C7F-AD3E-7D717801FA78}" name="Name"/>
     <tableColumn id="6" xr3:uid="{AC62AF06-F76A-42F0-9AB9-26210A66D70D}" name="PartName"/>
-    <tableColumn id="7" xr3:uid="{9DD94112-2513-41D3-B105-484B6645B3D9}" name="PartNumber" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{43EC1D7E-C868-40D2-9780-5F00D5F83130}" name="Fixture" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{88E7D7C9-E672-4CBE-8025-D3D11C725B19}" name="Manufactor" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{9DD94112-2513-41D3-B105-484B6645B3D9}" name="PartNumber" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{43EC1D7E-C868-40D2-9780-5F00D5F83130}" name="Fixture" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{88E7D7C9-E672-4CBE-8025-D3D11C725B19}" name="Manufactor" dataDxfId="0"/>
     <tableColumn id="9" xr3:uid="{558A41DA-0183-479A-9F7B-10588D343FE7}" name="Qty"/>
     <tableColumn id="11" xr3:uid="{27D41A9D-384B-41F8-842F-BB0D0F229DF2}" name="MultiFixture"/>
     <tableColumn id="10" xr3:uid="{D24942E5-5309-4DE5-9CD3-811BC95EAC83}" name="Notes"/>
+    <tableColumn id="13" xr3:uid="{060C349F-89F6-4B2B-AE5C-8959E269B6BF}" name="Pers"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1116,7 +1161,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10:M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2834,10 +2879,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC2EC58-D7C3-4E10-A80E-CCF958C566EE}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2847,9 +2892,11 @@
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2868,8 +2915,14 @@
       <c r="I1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>196</v>
+      </c>
+      <c r="N1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2888,8 +2941,14 @@
       <c r="I2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2908,8 +2967,14 @@
       <c r="I3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2928,8 +2993,14 @@
       <c r="I4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>3</v>
+      </c>
+      <c r="N4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2948,8 +3019,14 @@
       <c r="I5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>4</v>
+      </c>
+      <c r="N5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2968,8 +3045,14 @@
       <c r="I6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2988,8 +3071,14 @@
       <c r="I7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>6</v>
+      </c>
+      <c r="N7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3008,8 +3097,14 @@
       <c r="I8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>7</v>
+      </c>
+      <c r="N8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3028,8 +3123,14 @@
       <c r="I9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>8</v>
+      </c>
+      <c r="N9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3049,7 +3150,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F11">
         <v>10</v>
       </c>
@@ -3063,7 +3164,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F12">
         <v>11</v>
       </c>
@@ -3077,7 +3178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F13">
         <v>12</v>
       </c>
@@ -3091,7 +3192,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F14">
         <v>13</v>
       </c>
@@ -3105,7 +3206,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F15">
         <v>14</v>
       </c>
@@ -3119,7 +3220,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F16">
         <v>15</v>
       </c>
@@ -3283,19 +3384,20 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57924915-B8FC-4C0D-B0A4-CCA47CD6AE18}">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J50" sqref="J2:J50"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3310,7 +3412,7 @@
     <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>191</v>
       </c>
@@ -3347,14 +3449,17 @@
       <c r="L1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="3">
         <f ca="1">TODAY()</f>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C2" t="s">
         <v>194</v>
@@ -3383,14 +3488,17 @@
       <c r="K2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="3">
         <f t="shared" ref="B3:B12" ca="1" si="0">TODAY()</f>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C3" t="s">
         <v>194</v>
@@ -3419,14 +3527,17 @@
       <c r="K3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C4" t="s">
         <v>194</v>
@@ -3455,14 +3566,17 @@
       <c r="K4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C5" t="s">
         <v>194</v>
@@ -3491,14 +3605,17 @@
       <c r="K5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C6" t="s">
         <v>194</v>
@@ -3527,14 +3644,17 @@
       <c r="K6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C7" t="s">
         <v>194</v>
@@ -3563,14 +3683,17 @@
       <c r="K7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C8" t="s">
         <v>194</v>
@@ -3599,14 +3722,17 @@
       <c r="K8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C9" t="s">
         <v>194</v>
@@ -3635,14 +3761,17 @@
       <c r="K9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C10" t="s">
         <v>194</v>
@@ -3671,14 +3800,17 @@
       <c r="K10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C11" t="s">
         <v>194</v>
@@ -3707,14 +3839,17 @@
       <c r="K11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>194</v>
@@ -3744,14 +3879,17 @@
         <v>0</v>
       </c>
       <c r="L12" s="4"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13" s="5">
         <f ca="1">TODAY()</f>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>194</v>
@@ -3781,14 +3919,17 @@
         <v>0</v>
       </c>
       <c r="L13" s="4"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="3">
         <f t="shared" ref="B14:B16" ca="1" si="1">TODAY()</f>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>194</v>
@@ -3817,14 +3958,17 @@
       <c r="K14" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>194</v>
@@ -3853,14 +3997,17 @@
       <c r="K15" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>194</v>
@@ -3890,14 +4037,17 @@
         <v>0</v>
       </c>
       <c r="L16" s="4"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" s="5">
         <f ca="1">TODAY()</f>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>194</v>
@@ -3927,14 +4077,17 @@
         <v>0</v>
       </c>
       <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="3">
         <f t="shared" ref="B18:B22" ca="1" si="2">TODAY()</f>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>194</v>
@@ -3963,14 +4116,17 @@
       <c r="K18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>194</v>
@@ -3999,14 +4155,17 @@
       <c r="K19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>194</v>
@@ -4035,14 +4194,17 @@
       <c r="K20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>194</v>
@@ -4071,14 +4233,17 @@
       <c r="K21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
       <c r="B22" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>194</v>
@@ -4108,14 +4273,17 @@
         <v>0</v>
       </c>
       <c r="L22" s="4"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="3">
         <f t="shared" ref="B23:B25" ca="1" si="3">TODAY()</f>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>194</v>
@@ -4144,14 +4312,17 @@
       <c r="K23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
       <c r="B24" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>194</v>
@@ -4180,14 +4351,17 @@
       <c r="K24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>194</v>
@@ -4217,14 +4391,17 @@
         <v>0</v>
       </c>
       <c r="L25" s="4"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" s="5">
         <f ca="1">TODAY()</f>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>194</v>
@@ -4254,14 +4431,17 @@
         <v>1</v>
       </c>
       <c r="L26" s="4"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="3">
         <f t="shared" ref="B27:B33" ca="1" si="4">TODAY()</f>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>194</v>
@@ -4290,14 +4470,17 @@
       <c r="K27" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>194</v>
@@ -4326,14 +4509,17 @@
       <c r="K28" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>194</v>
@@ -4362,14 +4548,17 @@
       <c r="K29" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>29</v>
       </c>
       <c r="B30" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>194</v>
@@ -4398,14 +4587,17 @@
       <c r="K30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>194</v>
@@ -4434,14 +4626,17 @@
       <c r="K31" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>31</v>
       </c>
       <c r="B32" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>194</v>
@@ -4470,14 +4665,17 @@
       <c r="K32" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>194</v>
@@ -4507,14 +4705,17 @@
         <v>1</v>
       </c>
       <c r="L33" s="4"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>33</v>
       </c>
       <c r="B34" s="3">
         <f t="shared" ref="B34:B38" ca="1" si="5">TODAY()</f>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>194</v>
@@ -4543,14 +4744,17 @@
       <c r="K34" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>194</v>
@@ -4579,14 +4783,17 @@
       <c r="K35" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M35" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>35</v>
       </c>
       <c r="B36" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>194</v>
@@ -4615,14 +4822,17 @@
       <c r="K36" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>194</v>
@@ -4651,14 +4861,17 @@
       <c r="K37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>37</v>
       </c>
       <c r="B38" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>194</v>
@@ -4687,14 +4900,17 @@
       <c r="K38" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M38" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" s="3">
         <f t="shared" ref="B39:B50" ca="1" si="6">TODAY()</f>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>194</v>
@@ -4723,14 +4939,17 @@
       <c r="K39" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M39" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>39</v>
       </c>
       <c r="B40" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>194</v>
@@ -4759,14 +4978,17 @@
       <c r="K40" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M40" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>194</v>
@@ -4795,14 +5017,17 @@
       <c r="K41" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M41" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>41</v>
       </c>
       <c r="B42" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>194</v>
@@ -4831,14 +5056,17 @@
       <c r="K42" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M42" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>194</v>
@@ -4867,14 +5095,17 @@
       <c r="K43" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M43" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43</v>
       </c>
       <c r="B44" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>194</v>
@@ -4903,14 +5134,17 @@
       <c r="K44" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M44" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>194</v>
@@ -4939,14 +5173,17 @@
       <c r="K45" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M45" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>45</v>
       </c>
       <c r="B46" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>194</v>
@@ -4975,14 +5212,17 @@
       <c r="K46" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M46" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>194</v>
@@ -5011,14 +5251,17 @@
       <c r="K47" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M47" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>47</v>
       </c>
       <c r="B48" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>194</v>
@@ -5047,14 +5290,17 @@
       <c r="K48" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M48" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>194</v>
@@ -5083,14 +5329,17 @@
       <c r="K49" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M49" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>49</v>
       </c>
       <c r="B50" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>194</v>
@@ -5119,10 +5368,13 @@
       <c r="K50" t="b">
         <v>0</v>
       </c>
+      <c r="M50" t="s">
+        <v>199</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C50" xr:uid="{421CC119-A958-4092-B06A-C8B0915821FF}">
       <formula1>"IN,OUT"</formula1>
     </dataValidation>
@@ -5138,6 +5390,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I50" xr:uid="{CDBE01B2-841B-4AF2-B040-5CE26F81FDE3}">
       <formula1>INDIRECT("Manufactors[Manufactor]")</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M50" xr:uid="{57D22D2C-0D51-40A1-A560-A900279F418C}">
+      <formula1>INDIRECT("Personnel[Personnel]")</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>